<commit_message>
Revert: Merge remote-tracking branch 'origin/master'
</commit_message>
<xml_diff>
--- a/homework_03/excel_parse/table.xlsx
+++ b/homework_03/excel_parse/table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>RichardSmith</t>
+  </si>
+  <si>
+    <t>good@mail.com</t>
+  </si>
+  <si>
+    <t>asdсавыфа</t>
   </si>
 </sst>
 </file>
@@ -412,7 +418,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,6 +494,17 @@
         <v>43137</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43136</v>
+      </c>
+    </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
     </row>
@@ -498,8 +515,9 @@
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B6" r:id="rId4"/>
     <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>